<commit_message>
Hedging data saving process settled with 'export_hedging_data' function
</commit_message>
<xml_diff>
--- a/option_book_greeks_data.xlsx
+++ b/option_book_greeks_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours\MBA\Modélisation et langage fi\projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9090809-FBF8-4A0F-AF87-E6B3425E3F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A315D16F-8581-49BB-8894-3E0D2C1C58F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,192 +446,246 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="7" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>44940.796738356483</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>44940.796736111108</v>
+      </c>
+      <c r="B2">
+        <v>1.07</v>
       </c>
       <c r="C2">
+        <v>-0.49988311216195869</v>
+      </c>
+      <c r="D2">
+        <v>0.49450767852912231</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>44940.796747685177</v>
+      </c>
+      <c r="B3">
+        <v>1.0828</v>
+      </c>
+      <c r="C3">
+        <v>-0.52351885446815438</v>
+      </c>
+      <c r="D3">
+        <v>0.47087193622292661</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.05</v>
+      </c>
+      <c r="G3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>44940.798750000002</v>
+      </c>
+      <c r="B4">
         <v>1.07</v>
       </c>
-      <c r="D2">
+      <c r="C4">
         <v>-0.49988311216195869</v>
       </c>
-      <c r="E2">
+      <c r="D4">
         <v>0.49450767852912231</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>44940.79675277778</v>
-      </c>
-      <c r="C3">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>44940.798784722218</v>
+      </c>
+      <c r="B5">
         <v>1.0828</v>
       </c>
-      <c r="D3">
+      <c r="C5">
         <v>-0.52351885446815438</v>
       </c>
-      <c r="E3">
+      <c r="D5">
         <v>0.47087193622292661</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0.05</v>
-      </c>
-      <c r="H3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <v>44940.798748645837</v>
-      </c>
-      <c r="C4">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.05</v>
+      </c>
+      <c r="G5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>44940.802442129629</v>
+      </c>
+      <c r="B6">
         <v>1.07</v>
       </c>
-      <c r="D4">
+      <c r="C6">
         <v>-0.49988311216195869</v>
       </c>
-      <c r="E4">
+      <c r="D6">
         <v>0.49450767852912231</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2">
-        <v>44940.798782361111</v>
-      </c>
-      <c r="C5">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>44940.802453703713</v>
+      </c>
+      <c r="B7">
         <v>1.0828</v>
       </c>
-      <c r="D5">
+      <c r="C7">
         <v>-0.52351885446815438</v>
       </c>
-      <c r="E5">
+      <c r="D7">
         <v>0.47087193622292661</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0.05</v>
-      </c>
-      <c r="H5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2">
-        <v>44940.802439112027</v>
-      </c>
-      <c r="C6">
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.05</v>
+      </c>
+      <c r="G7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>44940.817280092589</v>
+      </c>
+      <c r="B8">
         <v>1.07</v>
       </c>
-      <c r="D6">
+      <c r="C8">
         <v>-0.49988311216195869</v>
       </c>
-      <c r="E6">
+      <c r="D8">
         <v>0.49450767852912231</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>44940.802450220472</v>
-      </c>
-      <c r="C7">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>44940.817326388889</v>
+      </c>
+      <c r="B9">
         <v>1.0828</v>
       </c>
-      <c r="D7">
+      <c r="C9">
         <v>-0.52351885446815438</v>
       </c>
-      <c r="E7">
+      <c r="D9">
         <v>0.47087193622292661</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0.05</v>
-      </c>
-      <c r="H7">
-        <v>0.05</v>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.05</v>
+      </c>
+      <c r="G9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>44941.45821759259</v>
+      </c>
+      <c r="B10">
+        <v>1.07</v>
+      </c>
+      <c r="C10">
+        <v>-0.49988311216195869</v>
+      </c>
+      <c r="D10">
+        <v>0.49450767852912231</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>